<commit_message>
Balans + Ultimate przycisk
</commit_message>
<xml_diff>
--- a/TArenaUnity3D/Assets/Resources/Data/Units.xlsx
+++ b/TArenaUnity3D/Assets/Resources/Data/Units.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\Unity\TArena\TArenaUnity3D\TArenaUnity3D\Assets\Resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wojtek\Documents\GitHub\TArenaUnity3D\Assets\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85EFB00-AFE4-45ED-BB84-BA6C95481552}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="32355" yWindow="645" windowWidth="26790" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toster_Arena" sheetId="1" r:id="rId1"/>
@@ -17,22 +18,28 @@
     <sheet name="Toster_Export_xml" sheetId="3" r:id="rId3"/>
     <sheet name="Spelle_Export_xml" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Piotr Musielski</author>
   </authors>
   <commentList>
-    <comment ref="M8" authorId="0" shapeId="0">
+    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0">
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0" shapeId="0">
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -154,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0" shapeId="0">
+    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -180,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB8" authorId="0" shapeId="0">
+    <comment ref="AB8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -228,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC8" authorId="0" shapeId="0">
+    <comment ref="AC8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -281,36 +288,36 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="mapowanie" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="mapowanie" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\piotr\Desktop\mapowanie.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" name="Units_Map" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="Units_Map" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\piotr\Desktop\Units_Map.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" name="Units_Map1" type="4" refreshedVersion="0" background="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="Units_Map1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\piotr\Desktop\Units_Map.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="4" name="Units_Mapping" type="4" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="Units_Mapping" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\piotr\Desktop\Units_Mapping.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="5" name="Units_Mapping_Template" type="4" refreshedVersion="0" background="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="Units_Mapping_Template" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\piotr\Desktop\Units_Mapping_Template.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="6" name="Units_Mapping_Template1" type="4" refreshedVersion="0" background="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="Units_Mapping_Template1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\piotr\Desktop\Units_Mapping_Template.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="7" name="Units_Mapping1" type="4" refreshedVersion="0" background="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="Units_Mapping1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\piotr\Desktop\Units_Mapping.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="8" name="Units_Mapping2" type="4" refreshedVersion="0" background="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="Units_Mapping2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\piotr\Desktop\Units_Mapping.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="272">
   <si>
     <t>Balans statystyk</t>
   </si>
@@ -1067,9 +1074,6 @@
     <t>ILOSC_ZLA</t>
   </si>
   <si>
-    <t>Kolumna5</t>
-  </si>
-  <si>
     <t>!ŚREDNIA</t>
   </si>
   <si>
@@ -1119,17 +1123,50 @@
   </si>
   <si>
     <t>Toughnessness</t>
+  </si>
+  <si>
+    <t>Golem</t>
+  </si>
+  <si>
+    <t>FixedAmountAfterSearching</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> w porównaniu do TosterHEAL</t>
+  </si>
+  <si>
+    <t>Ilość jednostki znaleziona przez symulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> w porównaniu do SuperLizard</t>
+  </si>
+  <si>
+    <t>FixedAmountAfterSearchingFixedAmountAfterSearching</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> w porównaniu do TosterDPS</t>
+  </si>
+  <si>
+    <t>ŚREDNIA</t>
+  </si>
+  <si>
+    <t>FixedAmountAfterSearchingFixedAmountAfterSearching2</t>
+  </si>
+  <si>
+    <t>CENA</t>
+  </si>
+  <si>
+    <t>Cena na podstawie średniej</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1284,8 +1321,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="115">
+  <fills count="116">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1970,6 +2015,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -2221,7 +2272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2746,9 +2797,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="105" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="111" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2773,51 +2821,62 @@
     <xf numFmtId="2" fontId="0" fillId="114" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="114" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="114" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="105" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="105" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="107" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="105" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="107" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="115" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="102" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="115" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="115" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="115" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="115" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="62">
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2864,156 +2923,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3031,494 +2941,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color rgb="FFCCCCCC"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3782,6 +3204,592 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="medium">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3840,141 +3848,146 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A8:AI25" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="53" tableBorderDxfId="54">
-  <autoFilter ref="A8:AI25"/>
-  <tableColumns count="35">
-    <tableColumn id="3" name="Name" dataDxfId="52"/>
-    <tableColumn id="1" name="S" dataDxfId="51"/>
-    <tableColumn id="2" name="I" dataDxfId="50"/>
-    <tableColumn id="4" name="Fraction" dataDxfId="18"/>
-    <tableColumn id="5" name="Level" dataDxfId="49"/>
-    <tableColumn id="10" name="Health" dataDxfId="19"/>
-    <tableColumn id="6" name="Attack" dataDxfId="48"/>
-    <tableColumn id="7" name="Defence" dataDxfId="47"/>
-    <tableColumn id="8" name="Damage min" dataDxfId="46"/>
-    <tableColumn id="9" name="Damage max" dataDxfId="45"/>
-    <tableColumn id="29" name="ZBALANSOWANA ILOSC" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A8:AL26" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59">
+  <autoFilter ref="A8:AL26" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="38">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="S" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="I" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fraction" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Level" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Health" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Attack" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Defence" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Damage min" dataDxfId="50"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Damage max" dataDxfId="49"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="ZBALANSOWANA ILOSC" dataDxfId="48">
       <calculatedColumnFormula>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="Toughnessness" dataDxfId="44">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Toughnessness" dataDxfId="47">
       <calculatedColumnFormula>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="VWO" dataDxfId="43">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="VWO" dataDxfId="46">
       <calculatedColumnFormula>AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$10)*IF(Tabela2[[#This Row],[Attack]]-$H$10 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$10 &gt; 0, $F$4,-$I$4)))/$F$10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="VWO_R" dataDxfId="42">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="VWO_R" dataDxfId="45">
       <calculatedColumnFormula>MAX(Tabela2[VWO])/Tabela2[[#This Row],[VWO]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="VWD" dataDxfId="41">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="VWD" dataDxfId="44">
       <calculatedColumnFormula>Tabela2[[#This Row],[Health]]/(AVERAGE($I$10,$J$10)*(1+($G$10-Tabela2[[#This Row],[Defence]])*IF($G$10-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$10-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="VWD_R" dataDxfId="40">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="VWD_R" dataDxfId="43">
       <calculatedColumnFormula>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="V_Off" dataDxfId="39">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="V_Off" dataDxfId="42">
       <calculatedColumnFormula>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="V_Def" dataDxfId="38">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="V_Def" dataDxfId="41">
       <calculatedColumnFormula>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" name="!ŚREDNIA" dataDxfId="37">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="!ŚREDNIA" dataDxfId="40">
       <calculatedColumnFormula>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" name="Odchyłka" dataDxfId="24">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Odchyłka" dataDxfId="39">
       <calculatedColumnFormula>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" name="Suma VW" dataDxfId="23">
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Suma VW" dataDxfId="38">
       <calculatedColumnFormula>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" name="Suma*Odchyłka" dataDxfId="36">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Suma*Odchyłka" dataDxfId="37">
       <calculatedColumnFormula>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" name="Kolumna2" dataDxfId="21">
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Kolumna2" dataDxfId="36">
       <calculatedColumnFormula>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="41" name="Kolumna1" dataDxfId="22">
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Kolumna1" dataDxfId="35">
       <calculatedColumnFormula>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" name="!Odchyłka" dataDxfId="35">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="!Odchyłka" dataDxfId="34">
       <calculatedColumnFormula>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="Cena_Atak" dataDxfId="34">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Cena_Atak" dataDxfId="33">
       <calculatedColumnFormula>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="Cena_Obrona" dataDxfId="33">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Cena_Obrona" dataDxfId="32">
       <calculatedColumnFormula>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="VOB" dataDxfId="32">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="VOB" dataDxfId="31">
       <calculatedColumnFormula>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="VDB" dataDxfId="31">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="VDB" dataDxfId="30">
       <calculatedColumnFormula>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="Cost1 (ZŁY)" dataDxfId="30">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Cost1 (ZŁY)" dataDxfId="29">
       <calculatedColumnFormula>INT(SQRT(((Tabela2[[#This Row],[VWO]])*Tabela2[[#This Row],[VWD]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="Stosunek W" dataDxfId="29">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Stosunek W" dataDxfId="28">
       <calculatedColumnFormula>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Stosunek B" dataDxfId="28">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Stosunek B" dataDxfId="27">
       <calculatedColumnFormula>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="CENA_ZLA" dataDxfId="27">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="CENA_ZLA" dataDxfId="26">
       <calculatedColumnFormula>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="ILOSC_ZLA" dataDxfId="26">
-      <calculatedColumnFormula>$AE$7/Tabela2[[#This Row],[Kolumna5]]</calculatedColumnFormula>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ILOSC_ZLA" dataDxfId="10">
+      <calculatedColumnFormula>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" name="Kolumna5" dataDxfId="25"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="FixedAmountAfterSearchingFixedAmountAfterSearching" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{E81D788C-D7EC-40FE-9AD7-435B0C143227}" name="FixedAmountAfterSearchingFixedAmountAfterSearching2" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{7DEC9FA1-82AC-4B54-B821-96FFC4B933A8}" name="FixedAmountAfterSearching" dataDxfId="1"/>
+    <tableColumn id="31" xr3:uid="{C3B58278-C645-4088-8882-E7DB32A0DDE7}" name="ŚREDNIA" dataDxfId="0">
+      <calculatedColumnFormula>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabela14" displayName="Tabela14" ref="B1:O7" tableType="xml" totalsRowShown="0" headerRowDxfId="70" connectionId="6">
-  <autoFilter ref="B1:O7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela14" displayName="Tabela14" ref="B1:O7" tableType="xml" totalsRowShown="0" headerRowDxfId="25" connectionId="6">
+  <autoFilter ref="B1:O7" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="69">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" uniqueName="Name" name="Name" dataDxfId="24">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="HP" name="HP" dataDxfId="68">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" uniqueName="HP" name="HP" dataDxfId="23">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/HP" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="Attack" name="A" dataDxfId="67">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" uniqueName="Attack" name="A" dataDxfId="22">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Attack" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="Defense" name="D" dataDxfId="66">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" uniqueName="Defense" name="D" dataDxfId="21">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Defense" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="Initiative" name="I" dataDxfId="65">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" uniqueName="Initiative" name="I" dataDxfId="20">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Initiative" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="Speed" name="S" dataDxfId="64">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" uniqueName="Speed" name="S" dataDxfId="19">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Speed" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="DamageMinimum" name="Dm" dataDxfId="63">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" uniqueName="DamageMinimum" name="Dm" dataDxfId="18">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/DamageMinimum" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="DamageMaximum" name="DM2" dataDxfId="62">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" uniqueName="DamageMaximum" name="DM2" dataDxfId="17">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/DamageMaximum" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="Cost" name="Cost" dataDxfId="61">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" uniqueName="Cost" name="Cost" dataDxfId="16">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Cost" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Skill1" name="Skill1" dataDxfId="60">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" uniqueName="Skill1" name="Skill1" dataDxfId="15">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Skills/Skill1" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="Skill2" name="Skill2" dataDxfId="59">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" uniqueName="Skill2" name="Skill2" dataDxfId="14">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Skills/Skill2" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="Skill3" name="Skill3" dataDxfId="58">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" uniqueName="Skill3" name="Skill3" dataDxfId="13">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Skills/Skill3" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="Skill4" name="Skill4" dataDxfId="57">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" uniqueName="Skill4" name="Skill4" dataDxfId="12">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Skills/Skill4" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="Sprite" name="Sprite" dataDxfId="56">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" uniqueName="Sprite" name="Sprite" dataDxfId="11">
       <xmlColumnPr mapId="8" xpath="/Units/Unit/Sprite" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -4244,14 +4257,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AO40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="AI13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomRight" activeCell="AU26" sqref="AU26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4275,10 +4288,11 @@
     <col min="26" max="27" width="3.7109375" style="169" hidden="1" customWidth="1"/>
     <col min="28" max="32" width="3.7109375" style="168" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="9.140625" customWidth="1"/>
-    <col min="34" max="34" width="9.85546875" style="220" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.85546875" style="219" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" s="153" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="150"/>
       <c r="B1" s="150"/>
       <c r="C1" s="151" t="s">
@@ -4300,7 +4314,7 @@
       <c r="Q1" s="200"/>
       <c r="R1" s="180"/>
       <c r="S1" s="207" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="T1" s="207"/>
       <c r="U1" s="207"/>
@@ -4317,9 +4331,18 @@
       <c r="AD1" s="168"/>
       <c r="AE1" s="168"/>
       <c r="AF1" s="170"/>
-      <c r="AH1" s="220"/>
+      <c r="AH1" s="219"/>
+      <c r="AI1" s="237" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ1" s="239"/>
+      <c r="AK1" s="239"/>
+      <c r="AL1" s="239"/>
+      <c r="AM1" s="239"/>
+      <c r="AN1" s="150"/>
+      <c r="AO1" s="237"/>
     </row>
-    <row r="2" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="160"/>
       <c r="B2" s="160"/>
       <c r="C2" s="160"/>
@@ -4331,7 +4354,7 @@
       <c r="I2" s="155"/>
       <c r="J2" s="155"/>
       <c r="L2" s="153" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M2" s="180"/>
       <c r="N2" s="187" t="s">
@@ -4343,7 +4366,7 @@
       <c r="R2" s="180"/>
       <c r="S2" s="207"/>
       <c r="T2" s="207" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="U2" s="207"/>
       <c r="V2" s="207"/>
@@ -4359,23 +4382,30 @@
       <c r="AD2" s="168"/>
       <c r="AE2" s="168"/>
       <c r="AF2" s="170"/>
-      <c r="AH2" s="220"/>
+      <c r="AH2" s="219"/>
+      <c r="AI2" s="237"/>
+      <c r="AJ2" s="239"/>
+      <c r="AK2" s="239"/>
+      <c r="AL2" s="239"/>
+      <c r="AM2" s="239"/>
+      <c r="AN2" s="150"/>
+      <c r="AO2" s="237"/>
     </row>
-    <row r="3" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="160"/>
       <c r="B3" s="160"/>
       <c r="C3" s="160"/>
       <c r="D3" s="160"/>
-      <c r="E3" s="214" t="s">
+      <c r="E3" s="236" t="s">
         <v>223</v>
       </c>
-      <c r="F3" s="214"/>
-      <c r="G3" s="214"/>
-      <c r="H3" s="214" t="s">
+      <c r="F3" s="236"/>
+      <c r="G3" s="236"/>
+      <c r="H3" s="236" t="s">
         <v>224</v>
       </c>
-      <c r="I3" s="214"/>
-      <c r="J3" s="214"/>
+      <c r="I3" s="236"/>
+      <c r="J3" s="236"/>
       <c r="M3" s="181"/>
       <c r="N3" s="180"/>
       <c r="O3" s="180" t="s">
@@ -4387,7 +4417,7 @@
       <c r="S3" s="207"/>
       <c r="T3" s="207"/>
       <c r="U3" s="207" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="V3" s="207"/>
       <c r="W3" s="207"/>
@@ -4400,9 +4430,18 @@
       <c r="AD3" s="168"/>
       <c r="AE3" s="168"/>
       <c r="AF3" s="168"/>
-      <c r="AH3" s="220"/>
+      <c r="AH3" s="219"/>
+      <c r="AI3" s="237" t="s">
+        <v>265</v>
+      </c>
+      <c r="AJ3" s="239"/>
+      <c r="AK3" s="239"/>
+      <c r="AL3" s="239"/>
+      <c r="AM3" s="239"/>
+      <c r="AN3" s="150"/>
+      <c r="AO3" s="237"/>
     </row>
-    <row r="4" spans="1:35" s="153" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" s="153" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="160"/>
       <c r="B4" s="160"/>
       <c r="C4" s="160"/>
@@ -4429,7 +4468,7 @@
       <c r="T4" s="207"/>
       <c r="U4" s="207"/>
       <c r="V4" s="207" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="W4" s="150"/>
       <c r="Y4" s="168"/>
@@ -4440,9 +4479,18 @@
       <c r="AD4" s="168"/>
       <c r="AE4" s="168"/>
       <c r="AF4" s="168"/>
-      <c r="AH4" s="220"/>
+      <c r="AH4" s="219"/>
+      <c r="AI4" s="237"/>
+      <c r="AJ4" s="239" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK4" s="239"/>
+      <c r="AL4" s="239"/>
+      <c r="AM4" s="239"/>
+      <c r="AN4" s="150"/>
+      <c r="AO4" s="237"/>
     </row>
-    <row r="5" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="162"/>
       <c r="B5" s="162"/>
       <c r="C5" s="162"/>
@@ -4466,7 +4514,7 @@
       <c r="U5" s="207"/>
       <c r="V5" s="207"/>
       <c r="W5" s="207" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Y5" s="168"/>
       <c r="Z5" s="169"/>
@@ -4476,9 +4524,18 @@
       <c r="AD5" s="168"/>
       <c r="AE5" s="168"/>
       <c r="AF5" s="168"/>
-      <c r="AH5" s="220"/>
+      <c r="AH5" s="219"/>
+      <c r="AI5" s="237"/>
+      <c r="AJ5" s="239"/>
+      <c r="AK5" s="239" t="s">
+        <v>267</v>
+      </c>
+      <c r="AL5" s="239"/>
+      <c r="AM5" s="239"/>
+      <c r="AN5" s="150"/>
+      <c r="AO5" s="237"/>
     </row>
-    <row r="6" spans="1:35" s="153" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" s="153" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="162"/>
       <c r="B6" s="162"/>
       <c r="C6" s="162"/>
@@ -4511,9 +4568,20 @@
       <c r="AD6" s="171"/>
       <c r="AE6" s="171"/>
       <c r="AF6" s="168"/>
-      <c r="AH6" s="220"/>
+      <c r="AH6" s="219"/>
+      <c r="AI6" s="237"/>
+      <c r="AJ6" s="239"/>
+      <c r="AK6" s="239"/>
+      <c r="AL6" s="239" t="s">
+        <v>268</v>
+      </c>
+      <c r="AM6" s="239"/>
+      <c r="AN6" s="150"/>
+      <c r="AO6" s="237" t="s">
+        <v>271</v>
+      </c>
     </row>
-    <row r="7" spans="1:35" s="157" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" s="157" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="162"/>
       <c r="B7" s="162"/>
       <c r="C7" s="162"/>
@@ -4547,11 +4615,11 @@
       </c>
       <c r="N7" s="191">
         <f>MAX(Tabela2[VWD])</f>
-        <v>796.17834394904469</v>
+        <v>547.77070063694282</v>
       </c>
       <c r="O7" s="196">
         <f>MAX(Tabela2[VOB])</f>
-        <v>796.1783439490448</v>
+        <v>547.77070063694271</v>
       </c>
       <c r="P7" s="158">
         <f>MAX(Tabela2[VDB])</f>
@@ -4559,7 +4627,7 @@
       </c>
       <c r="Q7" s="203">
         <f>MAX(Tabela2[Cost1 (ZŁY)])</f>
-        <v>343</v>
+        <v>284</v>
       </c>
       <c r="R7" s="204">
         <f>MAX(Tabela2[Stosunek W])</f>
@@ -4573,7 +4641,7 @@
       <c r="X7" s="172"/>
       <c r="Y7" s="172">
         <f>MAX(Tabela2[Stosunek B])</f>
-        <v>318.47133757961785</v>
+        <v>219.1082802547771</v>
       </c>
       <c r="Z7" s="173">
         <f>MAX(Tabela2[VWO_R])</f>
@@ -4581,11 +4649,11 @@
       </c>
       <c r="AA7" s="173">
         <f>MAX(Tabela2[VWD_R])</f>
-        <v>796.17834394904469</v>
+        <v>547.77070063694282</v>
       </c>
       <c r="AB7" s="173">
         <f>MAX(Tabela2[V_Off])</f>
-        <v>796.17834394904469</v>
+        <v>547.77070063694282</v>
       </c>
       <c r="AC7" s="173">
         <f>MAX(Tabela2[V_Def])</f>
@@ -4596,9 +4664,18 @@
         <v>5000</v>
       </c>
       <c r="AF7" s="173"/>
-      <c r="AH7" s="220"/>
+      <c r="AH7" s="219"/>
+      <c r="AI7" s="238">
+        <v>136</v>
+      </c>
+      <c r="AJ7" s="240">
+        <v>34550</v>
+      </c>
+      <c r="AK7" s="157">
+        <v>387</v>
+      </c>
     </row>
-    <row r="8" spans="1:35" s="147" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" s="147" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="147" t="s">
         <v>1</v>
       </c>
@@ -4629,23 +4706,23 @@
       <c r="J8" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="221" t="s">
-        <v>259</v>
+      <c r="K8" s="220" t="s">
+        <v>258</v>
       </c>
       <c r="L8" s="147" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M8" s="183" t="s">
+        <v>251</v>
+      </c>
+      <c r="N8" s="192" t="s">
+        <v>254</v>
+      </c>
+      <c r="O8" s="192" t="s">
         <v>252</v>
       </c>
-      <c r="N8" s="192" t="s">
-        <v>255</v>
-      </c>
-      <c r="O8" s="192" t="s">
+      <c r="P8" s="192" t="s">
         <v>253</v>
-      </c>
-      <c r="P8" s="192" t="s">
-        <v>254</v>
       </c>
       <c r="Q8" s="192" t="s">
         <v>235</v>
@@ -4654,16 +4731,16 @@
         <v>236</v>
       </c>
       <c r="S8" s="192" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T8" s="192" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="U8" s="192" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="V8" s="192" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="W8" s="188" t="s">
         <v>233</v>
@@ -4672,7 +4749,7 @@
         <v>227</v>
       </c>
       <c r="Y8" s="147" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Z8" s="179" t="s">
         <v>240</v>
@@ -4702,18 +4779,30 @@
         <v>243</v>
       </c>
       <c r="AI8" s="147" t="s">
-        <v>244</v>
+        <v>266</v>
+      </c>
+      <c r="AJ8" s="147" t="s">
+        <v>269</v>
+      </c>
+      <c r="AK8" s="147" t="s">
+        <v>262</v>
+      </c>
+      <c r="AL8" s="147" t="s">
+        <v>268</v>
+      </c>
+      <c r="AO8" s="242" t="s">
+        <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="141" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" s="141" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="141" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D9" s="141" t="s">
         <v>221</v>
       </c>
       <c r="F9" s="141">
-        <v>250</v>
+        <v>172</v>
       </c>
       <c r="G9" s="141">
         <v>50</v>
@@ -4727,13 +4816,13 @@
       <c r="J9" s="141">
         <v>50</v>
       </c>
-      <c r="K9" s="222">
+      <c r="K9" s="221">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>0.99952053140168862</v>
+        <v>1.3563745055921186</v>
       </c>
       <c r="L9" s="166">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
-        <v>5.3795834050611129</v>
+        <v>3.7011533826820462</v>
       </c>
       <c r="M9" s="184">
         <f>AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$10)*IF(Tabela2[[#This Row],[Attack]]-$H$10 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$10 &gt; 0, $F$4,-$I$4)))/$F$10</f>
@@ -4745,7 +4834,7 @@
       </c>
       <c r="O9" s="193">
         <f>Tabela2[[#This Row],[Health]]/(AVERAGE($I$10,$J$10)*(1+($G$10-Tabela2[[#This Row],[Defence]])*IF($G$10-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$10-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))</f>
-        <v>796.17834394904469</v>
+        <v>547.77070063694282</v>
       </c>
       <c r="P9" s="193">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
@@ -4757,35 +4846,35 @@
       </c>
       <c r="R9" s="193">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
-        <v>796.17834394904469</v>
+        <v>547.77070063694282</v>
       </c>
       <c r="S9" s="208">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>472.08917197452234</v>
+        <v>347.88535031847141</v>
       </c>
       <c r="T9" s="208">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.0000017539599015</v>
+        <v>1.3570275367095093</v>
       </c>
       <c r="U9" s="208">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
-        <v>944.17834394904469</v>
+        <v>695.77070063694282</v>
       </c>
       <c r="V9" s="208">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>944.17999999999984</v>
+        <v>944.18</v>
       </c>
       <c r="W9" s="213">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>552.34529999999984</v>
+        <v>552.34529999999995</v>
       </c>
       <c r="X9" s="208">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>0.99951877828583069</v>
+        <v>0.99951877828583047</v>
       </c>
       <c r="Y9" s="166">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>0.10002682254105619</v>
+        <v>7.3740834544053113E-2</v>
       </c>
       <c r="Z9" s="174">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
@@ -4797,35 +4886,55 @@
       </c>
       <c r="AB9" s="174">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>5</v>
+        <v>3.44</v>
       </c>
       <c r="AC9" s="174">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
-        <v>0.2</v>
+        <v>0.29069767441860467</v>
       </c>
       <c r="AD9" s="174">
         <f>INT(SQRT(((Tabela2[[#This Row],[VWO]])*Tabela2[[#This Row],[VWD]])))</f>
-        <v>343</v>
+        <v>284</v>
       </c>
       <c r="AE9" s="174">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
-        <v>5.3795834050611129</v>
+        <v>3.7011533826820462</v>
       </c>
       <c r="AF9" s="174">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>25</v>
+        <v>11.833599999999999</v>
       </c>
       <c r="AG9" s="174">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
         <v>2000</v>
       </c>
-      <c r="AH9" s="174" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI9" s="166"/>
+      <c r="AH9" s="174">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>40800</v>
+      </c>
+      <c r="AI9" s="243">
+        <v>136</v>
+      </c>
+      <c r="AJ9" s="243">
+        <v>136</v>
+      </c>
+      <c r="AK9" s="243">
+        <v>136</v>
+      </c>
+      <c r="AL9" s="243">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>136</v>
+      </c>
+      <c r="AN9" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>1</v>
+      </c>
+      <c r="AO9" s="141">
+        <f>1000/AN9</f>
+        <v>1000</v>
+      </c>
     </row>
-    <row r="10" spans="1:35" s="146" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" s="146" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="146" t="s">
         <v>189</v>
       </c>
@@ -4847,7 +4956,7 @@
       <c r="J10" s="146">
         <v>1</v>
       </c>
-      <c r="K10" s="223">
+      <c r="K10" s="222">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
         <v>471.86282004095767</v>
       </c>
@@ -4869,11 +4978,11 @@
       </c>
       <c r="P10" s="194">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>796.17834394904469</v>
+        <v>547.77070063694282</v>
       </c>
       <c r="Q10" s="194">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>796.17834394904469</v>
+        <v>547.77070063694282</v>
       </c>
       <c r="R10" s="194">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -4881,11 +4990,11 @@
       </c>
       <c r="S10" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>472.08917197452234</v>
+        <v>347.88535031847141</v>
       </c>
       <c r="T10" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.0000017539599015</v>
+        <v>1.3570275367095093</v>
       </c>
       <c r="U10" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -4893,23 +5002,23 @@
       </c>
       <c r="V10" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>2.0000035079198031</v>
+        <v>2.7140550734190185</v>
       </c>
       <c r="W10" s="212">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>1.1700020521330847</v>
+        <v>1.5877222179501258</v>
       </c>
       <c r="X10" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>471.86199241394394</v>
+        <v>347.71794033385669</v>
       </c>
       <c r="Y10" s="144">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>0.10002682254105619</v>
+        <v>7.3740834544053113E-2</v>
       </c>
       <c r="Z10" s="175">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>1.2559999999999998</v>
+        <v>1.8255813953488367</v>
       </c>
       <c r="AA10" s="175">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -4917,7 +5026,7 @@
       </c>
       <c r="AB10" s="175">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>796.1783439490448</v>
+        <v>547.77070063694271</v>
       </c>
       <c r="AC10" s="175">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -4933,19 +5042,39 @@
       </c>
       <c r="AF10" s="175">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>5.3795834050611138</v>
+        <v>3.7011533826820453</v>
       </c>
       <c r="AG10" s="175">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>8.0127567567567564</v>
-      </c>
-      <c r="AH10" s="175" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI10" s="144"/>
+        <v>8.5823381521055939</v>
+      </c>
+      <c r="AH10" s="175">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>10365000</v>
+      </c>
+      <c r="AI10" s="244">
+        <v>34550</v>
+      </c>
+      <c r="AJ10" s="244">
+        <v>34550</v>
+      </c>
+      <c r="AK10" s="243">
+        <v>33308</v>
+      </c>
+      <c r="AL10" s="243">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>34136</v>
+      </c>
+      <c r="AN10" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>251</v>
+      </c>
+      <c r="AO10" s="141">
+        <f t="shared" ref="AO10:AO26" si="0">1000/AN10</f>
+        <v>3.9840637450199203</v>
+      </c>
     </row>
-    <row r="11" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="139" t="s">
         <v>177</v>
       </c>
@@ -4972,9 +5101,9 @@
       <c r="J11" s="140">
         <v>60</v>
       </c>
-      <c r="K11" s="224">
+      <c r="K11" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>1.7525801559501779</v>
+        <v>1.7525801559501777</v>
       </c>
       <c r="L11" s="164">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
@@ -4994,11 +5123,11 @@
       </c>
       <c r="P11" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>1.7993630573248407</v>
+        <v>1.2379617834394907</v>
       </c>
       <c r="Q11" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>172.73885350318471</v>
+        <v>118.84433121019111</v>
       </c>
       <c r="R11" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -5006,11 +5135,11 @@
       </c>
       <c r="S11" s="210">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>427.44612291678413</v>
+        <v>400.49886177028736</v>
       </c>
       <c r="T11" s="210">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.1044432846380201</v>
+        <v>1.1787549105964124</v>
       </c>
       <c r="U11" s="210">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -5018,23 +5147,23 @@
       </c>
       <c r="V11" s="210">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>594.7182741916306</v>
+        <v>634.73344070770361</v>
       </c>
       <c r="W11" s="210">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>347.91019040210386</v>
+        <v>371.3190628140066</v>
       </c>
       <c r="X11" s="210">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>1.5868448659403853</v>
+        <v>1.4868062395289858</v>
       </c>
       <c r="Y11" s="164">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>9.0567799519805786E-2</v>
+        <v>8.4893256568143172E-2</v>
       </c>
       <c r="Z11" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>555.75221238938059</v>
+        <v>807.77937847293651</v>
       </c>
       <c r="AA11" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -5042,7 +5171,7 @@
       </c>
       <c r="AB11" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>7.8616352201257858</v>
+        <v>5.4088050314465406</v>
       </c>
       <c r="AC11" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -5058,19 +5187,33 @@
       </c>
       <c r="AF11" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>23.122456529781722</v>
+        <v>15.908250092489824</v>
       </c>
       <c r="AG11" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>1204.4008610380292</v>
-      </c>
-      <c r="AH11" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
+        <v>1456.4280271215853</v>
+      </c>
+      <c r="AH11" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="245"/>
+      <c r="AJ11" s="245"/>
+      <c r="AK11" s="143"/>
+      <c r="AL11" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>0</v>
+      </c>
+      <c r="AN11" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>0</v>
+      </c>
+      <c r="AO11" s="141" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AI11" s="165"/>
     </row>
-    <row r="12" spans="1:35" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="139" t="s">
         <v>38</v>
       </c>
@@ -5097,7 +5240,7 @@
       <c r="J12" s="137">
         <v>2</v>
       </c>
-      <c r="K12" s="224">
+      <c r="K12" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
         <v>150.38909982418647</v>
       </c>
@@ -5119,11 +5262,11 @@
       </c>
       <c r="P12" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>193.47133757961785</v>
+        <v>133.1082802547771</v>
       </c>
       <c r="Q12" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>417.89808917197456</v>
+        <v>287.51388535031856</v>
       </c>
       <c r="R12" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -5131,11 +5274,11 @@
       </c>
       <c r="S12" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>349.93365059116945</v>
+        <v>284.74154868034145</v>
       </c>
       <c r="T12" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.3490843169911282</v>
+        <v>1.657959655652435</v>
       </c>
       <c r="U12" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -5143,23 +5286,23 @@
       </c>
       <c r="V12" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>8.4658094374215285</v>
+        <v>10.404072097577306</v>
       </c>
       <c r="W12" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>4.9524985208915941</v>
+        <v>6.0863821770827231</v>
       </c>
       <c r="X12" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>111.47494484229146</v>
+        <v>90.707333746915467</v>
       </c>
       <c r="Y12" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>7.4144363494776142E-2</v>
+        <v>6.0356319718070171E-2</v>
       </c>
       <c r="Z12" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>5.1687242798353905</v>
+        <v>7.512680639295624</v>
       </c>
       <c r="AA12" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -5167,7 +5310,7 @@
       </c>
       <c r="AB12" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>365.49707602339186</v>
+        <v>251.46198830409358</v>
       </c>
       <c r="AC12" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -5183,19 +5326,33 @@
       </c>
       <c r="AF12" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>10.15269655620533</v>
+        <v>6.9850552306692659</v>
       </c>
       <c r="AG12" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>19.763318874429984</v>
-      </c>
-      <c r="AH12" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
+        <v>22.107275233890217</v>
+      </c>
+      <c r="AH12" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>0</v>
+      </c>
+      <c r="AI12" s="245"/>
+      <c r="AJ12" s="245"/>
+      <c r="AK12" s="143"/>
+      <c r="AL12" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>0</v>
+      </c>
+      <c r="AN12" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>0</v>
+      </c>
+      <c r="AO12" s="141" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AI12" s="165"/>
     </row>
-    <row r="13" spans="1:35" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" s="145" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="142" t="s">
         <v>217</v>
       </c>
@@ -5222,7 +5379,7 @@
       <c r="J13" s="143">
         <v>2</v>
       </c>
-      <c r="K13" s="224">
+      <c r="K13" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
         <v>99.113706927211737</v>
       </c>
@@ -5244,11 +5401,11 @@
       </c>
       <c r="P13" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>110.55505004549592</v>
+        <v>76.061874431301206</v>
       </c>
       <c r="Q13" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>256.48771610555053</v>
+        <v>176.46354868061877</v>
       </c>
       <c r="R13" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -5256,11 +5413,11 @@
       </c>
       <c r="S13" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>357.95153507845998</v>
+        <v>317.9394513659941</v>
       </c>
       <c r="T13" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.3188656947553579</v>
+        <v>1.4848424691296218</v>
       </c>
       <c r="U13" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -5268,23 +5425,23 @@
       </c>
       <c r="V13" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>12.557772386408052</v>
+        <v>14.138144491248369</v>
       </c>
       <c r="W13" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>7.3462968460487099</v>
+        <v>8.2708145273802955</v>
       </c>
       <c r="X13" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>75.150720290436226</v>
+        <v>66.750317954812914</v>
       </c>
       <c r="Y13" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>7.584320252006134E-2</v>
+        <v>6.7393238768875943E-2</v>
       </c>
       <c r="Z13" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>9.0452674897119323</v>
+        <v>13.147191118767344</v>
       </c>
       <c r="AA13" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -5292,7 +5449,7 @@
       </c>
       <c r="AB13" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>337.83783783783787</v>
+        <v>232.43243243243245</v>
       </c>
       <c r="AC13" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -5308,19 +5465,39 @@
       </c>
       <c r="AF13" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>16.422672672672672</v>
+        <v>11.298798798798799</v>
       </c>
       <c r="AG13" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>24.720943165387609</v>
-      </c>
-      <c r="AH13" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI13" s="165"/>
+        <v>28.822866794443019</v>
+      </c>
+      <c r="AH13" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>2709000</v>
+      </c>
+      <c r="AI13" s="245">
+        <v>9030</v>
+      </c>
+      <c r="AJ13" s="245">
+        <v>7472</v>
+      </c>
+      <c r="AK13" s="143">
+        <v>9080</v>
+      </c>
+      <c r="AL13" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>8527.3333333333339</v>
+      </c>
+      <c r="AN13" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>62.700980392156865</v>
+      </c>
+      <c r="AO13" s="141">
+        <f t="shared" si="0"/>
+        <v>15.948713939488702</v>
+      </c>
     </row>
-    <row r="14" spans="1:35" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" s="145" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="142" t="s">
         <v>219</v>
       </c>
@@ -5347,11 +5524,11 @@
       <c r="J14" s="149">
         <v>4</v>
       </c>
-      <c r="K14" s="224">
+      <c r="K14" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>47.01678938064947</v>
-      </c>
-      <c r="L14" s="219">
+        <v>47.016789380649485</v>
+      </c>
+      <c r="L14" s="218">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
         <v>3.3258833546189872</v>
       </c>
@@ -5369,11 +5546,11 @@
       </c>
       <c r="P14" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>51.592356687898089</v>
+        <v>35.49554140127389</v>
       </c>
       <c r="Q14" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>239.38853503184711</v>
+        <v>164.69931210191083</v>
       </c>
       <c r="R14" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -5381,11 +5558,11 @@
       </c>
       <c r="S14" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>365.80963575772859</v>
+        <v>328.46502429276046</v>
       </c>
       <c r="T14" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.2905346219820728</v>
+        <v>1.4372610935258263</v>
       </c>
       <c r="U14" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -5393,23 +5570,23 @@
       </c>
       <c r="V14" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>25.903738392633745</v>
+        <v>28.848846620963325</v>
       </c>
       <c r="W14" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>15.15368695969074</v>
+        <v>16.876575273263544</v>
       </c>
       <c r="X14" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>36.432024821184996</v>
+        <v>32.712768468051927</v>
       </c>
       <c r="Y14" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>7.7508186359591932E-2</v>
+        <v>6.9624331659000518E-2</v>
       </c>
       <c r="Z14" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>19.382716049382719</v>
+        <v>28.172552397358597</v>
       </c>
       <c r="AA14" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -5417,7 +5594,7 @@
       </c>
       <c r="AB14" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>168.91891891891893</v>
+        <v>116.21621621621622</v>
       </c>
       <c r="AC14" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -5433,19 +5610,39 @@
       </c>
       <c r="AF14" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>17.595720720720724</v>
+        <v>12.105855855855857</v>
       </c>
       <c r="AG14" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>50.73406740073407</v>
-      </c>
-      <c r="AH14" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI14" s="165"/>
+        <v>59.523903748709948</v>
+      </c>
+      <c r="AH14" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>1326300</v>
+      </c>
+      <c r="AI14" s="245">
+        <v>4421</v>
+      </c>
+      <c r="AJ14" s="245">
+        <v>3619</v>
+      </c>
+      <c r="AK14" s="143">
+        <v>4397</v>
+      </c>
+      <c r="AL14" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>4145.666666666667</v>
+      </c>
+      <c r="AN14" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>30.482843137254903</v>
+      </c>
+      <c r="AO14" s="141">
+        <f t="shared" si="0"/>
+        <v>32.805338908096807</v>
+      </c>
     </row>
-    <row r="15" spans="1:35" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" s="145" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="142" t="s">
         <v>220</v>
       </c>
@@ -5472,11 +5669,11 @@
       <c r="J15" s="143">
         <v>10</v>
       </c>
-      <c r="K15" s="224">
+      <c r="K15" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>12.798095913814294</v>
-      </c>
-      <c r="L15" s="219">
+        <v>12.798095913814292</v>
+      </c>
+      <c r="L15" s="218">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
         <v>3.7268932617769828</v>
       </c>
@@ -5494,11 +5691,11 @@
       </c>
       <c r="P15" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>13.694267515923567</v>
+        <v>9.4216560509554164</v>
       </c>
       <c r="Q15" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>213.63057324840767</v>
+        <v>146.97783439490451</v>
       </c>
       <c r="R15" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -5506,11 +5703,11 @@
       </c>
       <c r="S15" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>382.60538799570054</v>
+        <v>349.27901856894891</v>
       </c>
       <c r="T15" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.2338822578350752</v>
+        <v>1.3516128221335109</v>
       </c>
       <c r="U15" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -5518,23 +5715,23 @@
       </c>
       <c r="V15" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>90.985903794033874</v>
+        <v>99.667300846998529</v>
       </c>
       <c r="W15" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>53.226753719509816</v>
+        <v>58.305370995494137</v>
       </c>
       <c r="X15" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>10.372218120932677</v>
+        <v>9.4687588814173811</v>
       </c>
       <c r="Y15" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>8.1066890579653633E-2</v>
+        <v>7.4036248707867958E-2</v>
       </c>
       <c r="Z15" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>73.023255813953483</v>
+        <v>106.13845321795563</v>
       </c>
       <c r="AA15" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -5542,7 +5739,7 @@
       </c>
       <c r="AB15" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>49.019607843137258</v>
+        <v>33.725490196078432</v>
       </c>
       <c r="AC15" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -5558,19 +5755,39 @@
       </c>
       <c r="AF15" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>19.14828431372549</v>
+        <v>13.174019607843137</v>
       </c>
       <c r="AG15" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>178.4286612193589</v>
-      </c>
-      <c r="AH15" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI15" s="165"/>
+        <v>211.54385862336107</v>
+      </c>
+      <c r="AH15" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>371100</v>
+      </c>
+      <c r="AI15" s="245">
+        <v>1237</v>
+      </c>
+      <c r="AJ15" s="245">
+        <v>1035</v>
+      </c>
+      <c r="AK15" s="143">
+        <v>1291</v>
+      </c>
+      <c r="AL15" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>1187.6666666666667</v>
+      </c>
+      <c r="AN15" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>8.7328431372549034</v>
+      </c>
+      <c r="AO15" s="141">
+        <f t="shared" si="0"/>
+        <v>114.51024417625595</v>
+      </c>
     </row>
-    <row r="16" spans="1:35" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" s="145" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="142" t="s">
         <v>218</v>
       </c>
@@ -5597,11 +5814,11 @@
       <c r="J16" s="149">
         <v>24</v>
       </c>
-      <c r="K16" s="224">
+      <c r="K16" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
         <v>4.0983748493313668</v>
       </c>
-      <c r="L16" s="219">
+      <c r="L16" s="218">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
         <v>3.6127455670366113</v>
       </c>
@@ -5619,11 +5836,11 @@
       </c>
       <c r="P16" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>4.4146716450691859</v>
+        <v>3.0372940918076003</v>
       </c>
       <c r="Q16" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>220.38040852185375</v>
+        <v>151.62172106303541</v>
       </c>
       <c r="R16" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -5631,11 +5848,11 @@
       </c>
       <c r="S16" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>377.5333762216361</v>
+        <v>343.15403249222697</v>
       </c>
       <c r="T16" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.2504589785536024</v>
+        <v>1.3757378765778998</v>
       </c>
       <c r="U16" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -5643,23 +5860,23 @@
       </c>
       <c r="V16" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>287.94101157540621</v>
+        <v>316.7887652761263</v>
       </c>
       <c r="W16" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>168.44549177161261</v>
+        <v>185.32142768653387</v>
       </c>
       <c r="X16" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>3.277496439005084</v>
+        <v>2.9790375907407096</v>
       </c>
       <c r="Y16" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>7.9992226614096995E-2</v>
+        <v>7.2737942859533986E-2</v>
       </c>
       <c r="Z16" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>226.51741293532334</v>
+        <v>329.24042577808621</v>
       </c>
       <c r="AA16" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -5667,7 +5884,7 @@
       </c>
       <c r="AB16" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>15.052986512524086</v>
+        <v>10.356454720616572</v>
       </c>
       <c r="AC16" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -5683,19 +5900,39 @@
       </c>
       <c r="AF16" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>18.189025369299934</v>
+        <v>12.514049454078357</v>
       </c>
       <c r="AG16" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>563.81471023262066</v>
-      </c>
-      <c r="AH16" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI16" s="165"/>
+        <v>666.5377230753835</v>
+      </c>
+      <c r="AH16" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>115500</v>
+      </c>
+      <c r="AI16" s="245">
+        <v>385</v>
+      </c>
+      <c r="AJ16" s="245">
+        <v>326</v>
+      </c>
+      <c r="AK16" s="143">
+        <v>405</v>
+      </c>
+      <c r="AL16" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>372</v>
+      </c>
+      <c r="AN16" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>2.7352941176470589</v>
+      </c>
+      <c r="AO16" s="141">
+        <f t="shared" si="0"/>
+        <v>365.59139784946234</v>
+      </c>
     </row>
-    <row r="17" spans="1:35" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" s="145" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="142" t="s">
         <v>216</v>
       </c>
@@ -5722,7 +5959,7 @@
       <c r="J17" s="143">
         <v>2</v>
       </c>
-      <c r="K17" s="224">
+      <c r="K17" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
         <v>89.786872864641239</v>
       </c>
@@ -5744,11 +5981,11 @@
       </c>
       <c r="P17" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>95.342356687898089</v>
+        <v>65.595541401273891</v>
       </c>
       <c r="Q17" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>205.93949044585989</v>
+        <v>141.68636942675161</v>
       </c>
       <c r="R17" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -5756,11 +5993,11 @@
       </c>
       <c r="S17" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>389.05959289941649</v>
+        <v>356.93303238986238</v>
       </c>
       <c r="T17" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.2134130827666016</v>
+        <v>1.3226290568824592</v>
       </c>
       <c r="U17" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -5768,23 +6005,23 @@
       </c>
       <c r="V17" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>12.753858127390489</v>
+        <v>13.901797818251994</v>
       </c>
       <c r="W17" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>7.4610070045234353</v>
+        <v>8.1325517236774161</v>
       </c>
       <c r="X17" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>73.995306412821677</v>
+        <v>67.885150713591585</v>
       </c>
       <c r="Y17" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>8.2434415290816576E-2</v>
+        <v>7.5658660707249886E-2</v>
       </c>
       <c r="Z17" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>10.488517745302715</v>
+        <v>15.244938583288828</v>
       </c>
       <c r="AA17" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -5792,7 +6029,7 @@
       </c>
       <c r="AB17" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>365.49707602339186</v>
+        <v>251.46198830409358</v>
       </c>
       <c r="AC17" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -5808,19 +6045,39 @@
       </c>
       <c r="AF17" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>20.591384564698131</v>
+        <v>14.166872580512315</v>
       </c>
       <c r="AG17" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>25.083112339897308</v>
-      </c>
-      <c r="AH17" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI17" s="165"/>
+        <v>29.839533177883421</v>
+      </c>
+      <c r="AH17" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>2681700</v>
+      </c>
+      <c r="AI17" s="245">
+        <v>8939</v>
+      </c>
+      <c r="AJ17" s="245">
+        <v>7332</v>
+      </c>
+      <c r="AK17" s="245">
+        <v>8610</v>
+      </c>
+      <c r="AL17" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>8293.6666666666661</v>
+      </c>
+      <c r="AN17" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>60.982843137254896</v>
+      </c>
+      <c r="AO17" s="141">
+        <f t="shared" si="0"/>
+        <v>16.39805474056509</v>
+      </c>
     </row>
-    <row r="18" spans="1:35" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" s="145" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="142" t="s">
         <v>215</v>
       </c>
@@ -5847,9 +6104,9 @@
       <c r="J18" s="143">
         <v>3</v>
       </c>
-      <c r="K18" s="224">
+      <c r="K18" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>37.818519196630071</v>
+        <v>37.818519196630078</v>
       </c>
       <c r="L18" s="165">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
@@ -5869,11 +6126,11 @@
       </c>
       <c r="P18" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>36.464968152866248</v>
+        <v>25.087898089171979</v>
       </c>
       <c r="Q18" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>113.77070063694269</v>
+        <v>78.274242038216585</v>
       </c>
       <c r="R18" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -5881,11 +6138,11 @@
       </c>
       <c r="S18" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>574.744492631762</v>
+        <v>556.99626333239894</v>
       </c>
       <c r="T18" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>0.82139108082322654</v>
+        <v>0.84756403422812654</v>
       </c>
       <c r="U18" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -5893,23 +6150,23 @@
       </c>
       <c r="V18" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>20.497043246911407</v>
+        <v>21.1501647262705</v>
       </c>
       <c r="W18" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>11.990770299443172</v>
+        <v>12.372846364868241</v>
       </c>
       <c r="X18" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>46.042037805824535</v>
+        <v>44.620250116053192</v>
       </c>
       <c r="Y18" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>0.12177755556323</v>
+        <v>0.11806582041597809</v>
       </c>
       <c r="Z18" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>27.4235807860262</v>
+        <v>39.859855793642723</v>
       </c>
       <c r="AA18" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -5917,7 +6174,7 @@
       </c>
       <c r="AB18" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>254.06504065040653</v>
+        <v>174.79674796747972</v>
       </c>
       <c r="AC18" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -5933,19 +6190,39 @@
       </c>
       <c r="AF18" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>37.362505978000961</v>
+        <v>25.705404112864667</v>
       </c>
       <c r="AG18" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>48.504661867107288</v>
-      </c>
-      <c r="AH18" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI18" s="165"/>
+        <v>60.940936874723803</v>
+      </c>
+      <c r="AH18" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>1402800</v>
+      </c>
+      <c r="AI18" s="245">
+        <v>4676</v>
+      </c>
+      <c r="AJ18" s="245">
+        <v>3982</v>
+      </c>
+      <c r="AK18" s="143">
+        <v>4420</v>
+      </c>
+      <c r="AL18" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>4359.333333333333</v>
+      </c>
+      <c r="AN18" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>32.053921568627452</v>
+      </c>
+      <c r="AO18" s="141">
+        <f t="shared" si="0"/>
+        <v>31.197430799816484</v>
+      </c>
     </row>
-    <row r="19" spans="1:35" s="145" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" s="145" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="142" t="s">
         <v>214</v>
       </c>
@@ -5972,9 +6249,9 @@
       <c r="J19" s="143">
         <v>7</v>
       </c>
-      <c r="K19" s="224">
+      <c r="K19" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>16.618663282514984</v>
+        <v>16.618663282514987</v>
       </c>
       <c r="L19" s="165">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
@@ -5994,11 +6271,11 @@
       </c>
       <c r="P19" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>16.45435244161359</v>
+        <v>11.320594479830151</v>
       </c>
       <c r="Q19" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>138.21656050955417</v>
+        <v>95.092993630573275</v>
       </c>
       <c r="R19" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -6006,11 +6283,11 @@
       </c>
       <c r="S19" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>495.37556136076785</v>
+        <v>473.81377792127739</v>
       </c>
       <c r="T19" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>0.95299412571584319</v>
+        <v>0.99636190840874239</v>
       </c>
       <c r="U19" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -6018,23 +6295,23 @@
       </c>
       <c r="V19" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>54.117769642263561</v>
+        <v>56.580500114927425</v>
       </c>
       <c r="W19" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>31.658895240724181</v>
+        <v>33.099592567232541</v>
       </c>
       <c r="X19" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>17.438369066579341</v>
+        <v>16.679344264631833</v>
       </c>
       <c r="Y19" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>0.10496077078015205</v>
+        <v>0.10043373016541332</v>
       </c>
       <c r="Z19" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>60.774193548387082</v>
+        <v>88.334583645911451</v>
       </c>
       <c r="AA19" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -6042,7 +6319,7 @@
       </c>
       <c r="AB19" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>93.005952380952365</v>
+        <v>63.988095238095241</v>
       </c>
       <c r="AC19" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -6058,19 +6335,39 @@
       </c>
       <c r="AF19" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>30.328027950310553</v>
+        <v>20.865683229813666</v>
       </c>
       <c r="AG19" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>117.53095030514385</v>
-      </c>
-      <c r="AH19" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI19" s="165"/>
+        <v>145.09134040266821</v>
+      </c>
+      <c r="AH19" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>561600</v>
+      </c>
+      <c r="AI19" s="245">
+        <v>1872</v>
+      </c>
+      <c r="AJ19" s="245">
+        <v>1601</v>
+      </c>
+      <c r="AK19" s="143">
+        <v>1865</v>
+      </c>
+      <c r="AL19" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>1779.3333333333333</v>
+      </c>
+      <c r="AN19" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>13.083333333333332</v>
+      </c>
+      <c r="AO19" s="141">
+        <f t="shared" si="0"/>
+        <v>76.433121019108285</v>
+      </c>
     </row>
-    <row r="20" spans="1:35" s="145" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" s="145" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="142" t="s">
         <v>213</v>
       </c>
@@ -6097,7 +6394,7 @@
       <c r="J20" s="149">
         <v>16</v>
       </c>
-      <c r="K20" s="224">
+      <c r="K20" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
         <v>4.00445615147349</v>
       </c>
@@ -6119,11 +6416,11 @@
       </c>
       <c r="P20" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>3.7444508782088408</v>
+        <v>2.576182204207683</v>
       </c>
       <c r="Q20" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>86.272148233931688</v>
+        <v>59.355237984945013</v>
       </c>
       <c r="R20" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -6131,11 +6428,11 @@
       </c>
       <c r="S20" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>726.05864714102074</v>
+        <v>712.60019201652744</v>
       </c>
       <c r="T20" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>0.65020918332001765</v>
+        <v>0.66248929664763645</v>
       </c>
       <c r="U20" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -6143,23 +6440,23 @@
       </c>
       <c r="V20" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>153.23406088240827</v>
+        <v>156.1281012644265</v>
       </c>
       <c r="W20" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>89.641925616208837</v>
+        <v>91.334939239689504</v>
       </c>
       <c r="X20" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>6.1587197692693785</v>
+        <v>6.0445597713609134</v>
       </c>
       <c r="Y20" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>0.15383818092716953</v>
+        <v>0.15104899590467505</v>
       </c>
       <c r="Z20" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>267.06185567010306</v>
+        <v>388.17130184607987</v>
       </c>
       <c r="AA20" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -6167,7 +6464,7 @@
       </c>
       <c r="AB20" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>33.386752136752136</v>
+        <v>22.970085470085472</v>
       </c>
       <c r="AC20" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -6183,19 +6480,39 @@
       </c>
       <c r="AF20" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>47.489776746242256</v>
+        <v>32.672966401414676</v>
       </c>
       <c r="AG20" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>422.73753134577873</v>
-      </c>
-      <c r="AH20" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI20" s="165"/>
+        <v>543.84697752175555</v>
+      </c>
+      <c r="AH20" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>163200</v>
+      </c>
+      <c r="AI20" s="245">
+        <v>544</v>
+      </c>
+      <c r="AJ20" s="245">
+        <v>477</v>
+      </c>
+      <c r="AK20" s="143">
+        <v>538</v>
+      </c>
+      <c r="AL20" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>519.66666666666663</v>
+      </c>
+      <c r="AN20" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>3.8210784313725488</v>
+      </c>
+      <c r="AO20" s="141">
+        <f t="shared" si="0"/>
+        <v>261.70622193713922</v>
+      </c>
     </row>
-    <row r="21" spans="1:35" s="145" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" s="145" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="142" t="s">
         <v>190</v>
       </c>
@@ -6220,9 +6537,9 @@
       <c r="J21" s="143">
         <v>13</v>
       </c>
-      <c r="K21" s="224">
+      <c r="K21" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>14.878662749208166</v>
+        <v>14.878662749208168</v>
       </c>
       <c r="L21" s="165">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
@@ -6242,11 +6559,11 @@
       </c>
       <c r="P21" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>18.232484076433124</v>
+        <v>12.54394904458599</v>
       </c>
       <c r="Q21" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>360.27388535031855</v>
+        <v>247.86843312101917</v>
       </c>
       <c r="R21" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -6254,11 +6571,11 @@
       </c>
       <c r="S21" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>343.67140866883005</v>
+        <v>287.46868255418036</v>
       </c>
       <c r="T21" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.3736667877859956</v>
+        <v>1.6422310625472161</v>
       </c>
       <c r="U21" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -6266,23 +6583,23 @@
       </c>
       <c r="V21" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>87.129104974948035</v>
+        <v>104.16363263205596</v>
       </c>
       <c r="W21" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>50.970526410344597</v>
+        <v>60.935725089752736</v>
       </c>
       <c r="X21" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>10.831347806835177</v>
+        <v>9.060030033855476</v>
       </c>
       <c r="Y21" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>7.2817512131388359E-2</v>
+        <v>6.0934386968059688E-2</v>
       </c>
       <c r="Z21" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>54.8471615720524</v>
+        <v>79.71971158728546</v>
       </c>
       <c r="AA21" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -6290,7 +6607,7 @@
       </c>
       <c r="AB21" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>38.771712158808931</v>
+        <v>26.674937965260547</v>
       </c>
       <c r="AC21" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -6306,19 +6623,39 @@
       </c>
       <c r="AF21" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>11.403444752590863</v>
+        <v>7.845569989782514</v>
       </c>
       <c r="AG21" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>188.3606750855659</v>
-      </c>
-      <c r="AH21" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI21" s="165"/>
+        <v>213.23322510079896</v>
+      </c>
+      <c r="AH21" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>365100</v>
+      </c>
+      <c r="AI21" s="245">
+        <v>1217</v>
+      </c>
+      <c r="AJ21" s="245">
+        <v>1233</v>
+      </c>
+      <c r="AK21" s="143">
+        <v>1315</v>
+      </c>
+      <c r="AL21" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>1255</v>
+      </c>
+      <c r="AN21" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>9.2279411764705888</v>
+      </c>
+      <c r="AO21" s="141">
+        <f t="shared" si="0"/>
+        <v>108.36653386454182</v>
+      </c>
     </row>
-    <row r="22" spans="1:35" s="145" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" s="145" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="142" t="s">
         <v>191</v>
       </c>
@@ -6343,9 +6680,9 @@
       <c r="J22" s="149">
         <v>11</v>
       </c>
-      <c r="K22" s="224">
+      <c r="K22" s="223">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>12.268807281048844</v>
+        <v>12.268807281048847</v>
       </c>
       <c r="L22" s="165">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
@@ -6365,11 +6702,11 @@
       </c>
       <c r="P22" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>13.129431558706887</v>
+        <v>9.0330489123903401</v>
       </c>
       <c r="Q22" s="201">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>213.74714577574815</v>
+        <v>147.05803629371474</v>
       </c>
       <c r="R22" s="205">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
@@ -6377,11 +6714,11 @@
       </c>
       <c r="S22" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>382.51326500353866</v>
+        <v>349.16871026252198</v>
       </c>
       <c r="T22" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.2341794211911385</v>
+        <v>1.3520398195046166</v>
       </c>
       <c r="U22" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -6389,23 +6726,23 @@
       </c>
       <c r="V22" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>94.933984824966956</v>
+        <v>103.99989296833684</v>
       </c>
       <c r="W22" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>55.536381122605668</v>
+        <v>60.839937386477047</v>
       </c>
       <c r="X22" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>9.9408619771085629</v>
+        <v>9.0742943396031794</v>
       </c>
       <c r="Y22" s="165">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>8.1047371449082625E-2</v>
+        <v>7.4012866790332144E-2</v>
       </c>
       <c r="Z22" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>76.164759725400444</v>
+        <v>110.70459262412855</v>
       </c>
       <c r="AA22" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -6413,7 +6750,7 @@
       </c>
       <c r="AB22" s="176">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>47.15201810637496</v>
+        <v>32.440588457185967</v>
       </c>
       <c r="AC22" s="176">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -6429,24 +6766,44 @@
       </c>
       <c r="AF22" s="178">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>19.223515074137485</v>
+        <v>13.225778371006587</v>
       </c>
       <c r="AG22" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>186.16475972540047</v>
-      </c>
-      <c r="AH22" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI22" s="165"/>
+        <v>220.70459262412857</v>
+      </c>
+      <c r="AH22" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>354600</v>
+      </c>
+      <c r="AI22" s="245">
+        <v>1182</v>
+      </c>
+      <c r="AJ22" s="245">
+        <v>982</v>
+      </c>
+      <c r="AK22" s="143">
+        <v>1217</v>
+      </c>
+      <c r="AL22" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>1127</v>
+      </c>
+      <c r="AN22" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>8.2867647058823533</v>
+      </c>
+      <c r="AO22" s="141">
+        <f t="shared" si="0"/>
+        <v>120.67435669920141</v>
+      </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="136" t="s">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A23" s="241" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="218"/>
-      <c r="C23" s="218"/>
+      <c r="B23" s="217"/>
+      <c r="C23" s="217"/>
       <c r="D23" s="136" t="s">
         <v>221</v>
       </c>
@@ -6466,15 +6823,15 @@
       <c r="J23" s="137">
         <v>25</v>
       </c>
-      <c r="K23" s="225">
+      <c r="K23" s="224">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>3.9777182676619431</v>
-      </c>
-      <c r="L23" s="215">
+        <v>3.9777182676619427</v>
+      </c>
+      <c r="L23" s="214">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
         <v>3.8418982050651591</v>
       </c>
-      <c r="M23" s="216">
+      <c r="M23" s="215">
         <f>AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$10)*IF(Tabela2[[#This Row],[Attack]]-$H$10 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$10 &gt; 0, $F$4,-$I$4)))/$F$10</f>
         <v>49</v>
       </c>
@@ -6488,23 +6845,23 @@
       </c>
       <c r="P23" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>4.2292993630573248</v>
+        <v>2.9097579617834399</v>
       </c>
       <c r="Q23" s="209">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>207.23566878980893</v>
-      </c>
-      <c r="R23" s="217">
+        <v>142.57814012738856</v>
+      </c>
+      <c r="R23" s="216">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
         <v>568.60093434964358</v>
       </c>
       <c r="S23" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>387.91830156972628</v>
+        <v>355.58953723851607</v>
       </c>
       <c r="T23" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.2169830556838119</v>
+        <v>1.32762623913577</v>
       </c>
       <c r="U23" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -6512,23 +6869,23 @@
       </c>
       <c r="V23" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>288.7328955725979</v>
+        <v>314.98332410917573</v>
       </c>
       <c r="W23" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>168.90874390996976</v>
+        <v>184.26524460386779</v>
       </c>
       <c r="X23" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>3.2685075187237498</v>
-      </c>
-      <c r="Y23" s="219">
+        <v>2.9961130251924466</v>
+      </c>
+      <c r="Y23" s="218">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>8.2192597108829701E-2</v>
+        <v>7.5373881674228024E-2</v>
       </c>
       <c r="Z23" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>236.44578313253012</v>
+        <v>343.67119641356112</v>
       </c>
       <c r="AA23" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -6536,7 +6893,7 @@
       </c>
       <c r="AB23" s="144">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>15.384615384615387</v>
+        <v>10.584615384615388</v>
       </c>
       <c r="AC23" s="144">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -6550,149 +6907,189 @@
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
         <v>3.8418982050651591</v>
       </c>
-      <c r="AF23" s="219">
+      <c r="AF23" s="218">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>19.230769230769234</v>
+        <v>13.230769230769234</v>
       </c>
       <c r="AG23" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>567.52686421361125</v>
-      </c>
-      <c r="AH23" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI23" s="219"/>
+        <v>674.75227749464216</v>
+      </c>
+      <c r="AH23" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>116100</v>
+      </c>
+      <c r="AI23" s="246">
+        <v>387</v>
+      </c>
+      <c r="AJ23" s="247">
+        <v>387</v>
+      </c>
+      <c r="AK23" s="243">
+        <v>387</v>
+      </c>
+      <c r="AL23" s="243">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>387</v>
+      </c>
+      <c r="AN23" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>2.8455882352941178</v>
+      </c>
+      <c r="AO23" s="141">
+        <f t="shared" si="0"/>
+        <v>351.42118863049092</v>
+      </c>
     </row>
-    <row r="24" spans="1:35" s="236" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="227" t="s">
+    <row r="24" spans="1:41" s="235" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="226" t="s">
         <v>188</v>
       </c>
-      <c r="B24" s="228"/>
-      <c r="C24" s="228"/>
-      <c r="D24" s="227" t="s">
+      <c r="B24" s="227"/>
+      <c r="C24" s="227"/>
+      <c r="D24" s="226" t="s">
         <v>221</v>
       </c>
-      <c r="E24" s="229"/>
-      <c r="F24" s="229">
+      <c r="E24" s="228"/>
+      <c r="F24" s="228">
         <v>100</v>
       </c>
-      <c r="G24" s="229">
+      <c r="G24" s="228">
         <v>1</v>
       </c>
-      <c r="H24" s="229">
+      <c r="H24" s="228">
         <v>50</v>
       </c>
-      <c r="I24" s="229">
+      <c r="I24" s="228">
         <v>5</v>
       </c>
-      <c r="J24" s="229">
+      <c r="J24" s="228">
         <v>5</v>
       </c>
-      <c r="K24" s="230">
+      <c r="K24" s="229">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>2.9174938563130977</v>
-      </c>
-      <c r="L24" s="231">
+        <v>2.9174938563130981</v>
+      </c>
+      <c r="L24" s="230">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
         <v>63.694267515923585</v>
       </c>
-      <c r="M24" s="232">
+      <c r="M24" s="231">
         <f>AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$10)*IF(Tabela2[[#This Row],[Attack]]-$H$10 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$10 &gt; 0, $F$4,-$I$4)))/$F$10</f>
         <v>5</v>
       </c>
-      <c r="N24" s="233">
+      <c r="N24" s="232">
         <f>MAX(Tabela2[VWO])/Tabela2[[#This Row],[VWO]]</f>
         <v>29.6</v>
       </c>
-      <c r="O24" s="233">
+      <c r="O24" s="232">
         <f>Tabela2[[#This Row],[Health]]/(AVERAGE($I$10,$J$10)*(1+($G$10-Tabela2[[#This Row],[Defence]])*IF($G$10-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$10-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))</f>
         <v>318.47133757961791</v>
       </c>
-      <c r="P24" s="233">
+      <c r="P24" s="232">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>2.4999999999999996</v>
-      </c>
-      <c r="Q24" s="230">
+        <v>1.72</v>
+      </c>
+      <c r="Q24" s="229">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>12.499999999999998</v>
-      </c>
-      <c r="R24" s="234">
+        <v>8.6</v>
+      </c>
+      <c r="R24" s="233">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
         <v>9426.7515923566898</v>
       </c>
-      <c r="S24" s="233">
+      <c r="S24" s="232">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>4719.6257961783449</v>
-      </c>
-      <c r="T24" s="233">
+        <v>4717.6757961783451</v>
+      </c>
+      <c r="T24" s="232">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>0.10002699798409201</v>
-      </c>
-      <c r="U24" s="233">
+        <v>0.10006834305621989</v>
+      </c>
+      <c r="U24" s="232">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
         <v>323.47133757961791</v>
       </c>
-      <c r="V24" s="233">
+      <c r="V24" s="232">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>32.355866831987989</v>
-      </c>
-      <c r="W24" s="233">
+        <v>32.369240777771516</v>
+      </c>
+      <c r="W24" s="232">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>18.928182096712973</v>
-      </c>
-      <c r="X24" s="233">
+        <v>18.936005854996335</v>
+      </c>
+      <c r="X24" s="232">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>29.167064043820318</v>
-      </c>
-      <c r="Y24" s="230">
+        <v>29.155013136112451</v>
+      </c>
+      <c r="Y24" s="229">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
         <v>1</v>
       </c>
-      <c r="Z24" s="232">
+      <c r="Z24" s="231">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>400.00000000000006</v>
-      </c>
-      <c r="AA24" s="232">
+        <v>581.39534883720933</v>
+      </c>
+      <c r="AA24" s="231">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
         <v>33.783783783783782</v>
       </c>
-      <c r="AB24" s="232">
+      <c r="AB24" s="231">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>159.23566878980893</v>
-      </c>
-      <c r="AC24" s="232">
+        <v>109.55414012738855</v>
+      </c>
+      <c r="AC24" s="231">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
         <v>0.5</v>
       </c>
-      <c r="AD24" s="235">
+      <c r="AD24" s="234">
         <f>INT(SQRT(((Tabela2[[#This Row],[VWO]])*Tabela2[[#This Row],[VWD]])))</f>
         <v>39</v>
       </c>
-      <c r="AE24" s="232">
+      <c r="AE24" s="231">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
         <v>63.694267515923585</v>
       </c>
-      <c r="AF24" s="230">
+      <c r="AF24" s="229">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>318.47133757961785</v>
-      </c>
-      <c r="AG24" s="232">
+        <v>219.1082802547771</v>
+      </c>
+      <c r="AG24" s="231">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>433.78378378378386</v>
-      </c>
-      <c r="AH24" s="232" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI24" s="230"/>
+        <v>615.17913262099307</v>
+      </c>
+      <c r="AH24" s="231">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>303900</v>
+      </c>
+      <c r="AI24" s="245">
+        <v>1013</v>
+      </c>
+      <c r="AJ24" s="245">
+        <v>860</v>
+      </c>
+      <c r="AK24" s="143">
+        <v>958</v>
+      </c>
+      <c r="AL24" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>943.66666666666663</v>
+      </c>
+      <c r="AN24" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>6.9387254901960782</v>
+      </c>
+      <c r="AO24" s="141">
+        <f t="shared" si="0"/>
+        <v>144.11868597668669</v>
+      </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="136" t="s">
         <v>192</v>
       </c>
-      <c r="B25" s="218"/>
-      <c r="C25" s="218"/>
+      <c r="B25" s="217"/>
+      <c r="C25" s="217"/>
       <c r="D25" s="136" t="s">
         <v>221</v>
       </c>
@@ -6712,15 +7109,15 @@
       <c r="J25" s="137">
         <v>9</v>
       </c>
-      <c r="K25" s="225">
+      <c r="K25" s="224">
         <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
         <v>12.345810315354626</v>
       </c>
-      <c r="L25" s="215">
+      <c r="L25" s="214">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
         <v>3.7185780157667714</v>
       </c>
-      <c r="M25" s="216">
+      <c r="M25" s="215">
         <f>AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$10)*IF(Tabela2[[#This Row],[Attack]]-$H$10 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$10 &gt; 0, $F$4,-$I$4)))/$F$10</f>
         <v>16.2</v>
       </c>
@@ -6734,23 +7131,23 @@
       </c>
       <c r="P25" s="198">
         <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
-        <v>13.216560509554139</v>
-      </c>
-      <c r="Q25" s="219">
+        <v>9.0929936305732486</v>
+      </c>
+      <c r="Q25" s="218">
         <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
-        <v>214.10828025477704</v>
-      </c>
-      <c r="R25" s="226">
+        <v>147.30649681528661</v>
+      </c>
+      <c r="R25" s="225">
         <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
         <v>550.34954633348218</v>
       </c>
       <c r="S25" s="209">
         <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
-        <v>382.2289132941296</v>
+        <v>348.82802157438437</v>
       </c>
       <c r="T25" s="209">
         <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
-        <v>1.2350975647850093</v>
+        <v>1.3533603116782036</v>
       </c>
       <c r="U25" s="209">
         <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
@@ -6758,23 +7155,23 @@
       </c>
       <c r="V25" s="209">
         <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
-        <v>94.412048307650252</v>
+        <v>103.4521666683558</v>
       </c>
       <c r="W25" s="209">
         <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
-        <v>55.231048259975395</v>
+        <v>60.519517500988137</v>
       </c>
       <c r="X25" s="209">
         <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
-        <v>9.9958178749252369</v>
-      </c>
-      <c r="Y25" s="219">
+        <v>9.1223380860382157</v>
+      </c>
+      <c r="Y25" s="218">
         <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
-        <v>8.0987122666300038E-2</v>
+        <v>7.3940651423516648E-2</v>
       </c>
       <c r="Z25" s="176">
         <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
-        <v>75.662650602409641</v>
+        <v>109.9747828523396</v>
       </c>
       <c r="AA25" s="176">
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
@@ -6782,7 +7179,7 @@
       </c>
       <c r="AB25" s="144">
         <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
-        <v>46.763935652824543</v>
+        <v>32.173587729143286</v>
       </c>
       <c r="AC25" s="144">
         <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
@@ -6796,33 +7193,181 @@
         <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
         <v>3.7185780157667714</v>
       </c>
-      <c r="AF25" s="219">
+      <c r="AF25" s="218">
         <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
-        <v>18.705574261129819</v>
+        <v>12.869435091657314</v>
       </c>
       <c r="AG25" s="176">
         <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
-        <v>185.12211006186908</v>
-      </c>
-      <c r="AH25" s="176" t="e">
-        <f>$AE$7/Tabela2[[#This Row],[Kolumna5]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AI25" s="219"/>
+        <v>219.43424231179904</v>
+      </c>
+      <c r="AH25" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>358800</v>
+      </c>
+      <c r="AI25" s="248">
+        <v>1196</v>
+      </c>
+      <c r="AJ25" s="245">
+        <v>999</v>
+      </c>
+      <c r="AK25" s="143">
+        <v>1162</v>
+      </c>
+      <c r="AL25" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>1119</v>
+      </c>
+      <c r="AN25" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>8.2279411764705888</v>
+      </c>
+      <c r="AO25" s="141">
+        <f t="shared" si="0"/>
+        <v>121.53708668453976</v>
+      </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A26" s="135"/>
-      <c r="B26" s="135"/>
-      <c r="C26" s="135"/>
-      <c r="D26" s="135"/>
-      <c r="E26" s="135"/>
-      <c r="F26" s="135"/>
-      <c r="G26" s="135"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="135"/>
-      <c r="J26" s="135"/>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A26" s="136" t="s">
+        <v>261</v>
+      </c>
+      <c r="B26" s="142"/>
+      <c r="C26" s="142"/>
+      <c r="E26" s="137"/>
+      <c r="F26" s="137">
+        <v>30</v>
+      </c>
+      <c r="G26" s="137">
+        <v>7</v>
+      </c>
+      <c r="H26" s="137">
+        <v>10</v>
+      </c>
+      <c r="I26" s="137">
+        <v>4</v>
+      </c>
+      <c r="J26" s="137">
+        <v>4</v>
+      </c>
+      <c r="K26" s="224">
+        <f>Tabela2[[#This Row],[Kolumna1]]*Tabela2[[#This Row],[Odchyłka]]</f>
+        <v>24.022578958160349</v>
+      </c>
+      <c r="L26" s="214">
+        <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
+        <v>6.9203513693068572</v>
+      </c>
+      <c r="M26" s="215">
+        <f>AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$10)*IF(Tabela2[[#This Row],[Attack]]-$H$10 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$10 &gt; 0, $F$4,-$I$4)))/$F$10</f>
+        <v>4.96</v>
+      </c>
+      <c r="N26" s="189">
+        <f>MAX(Tabela2[VWO])/Tabela2[[#This Row],[VWO]]</f>
+        <v>29.838709677419356</v>
+      </c>
+      <c r="O26" s="197">
+        <f>Tabela2[[#This Row],[Health]]/(AVERAGE($I$10,$J$10)*(1+($G$10-Tabela2[[#This Row],[Defence]])*IF($G$10-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$10-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))</f>
+        <v>34.324942791762012</v>
+      </c>
+      <c r="P26" s="198">
+        <f>MAX(Tabela2[VWD])/Tabela2[[#This Row],[VWD]]</f>
+        <v>15.958386411889601</v>
+      </c>
+      <c r="Q26" s="218">
+        <f>Tabela2[[#This Row],[VWO]]*Tabela2[[#This Row],[VWD_R]]</f>
+        <v>79.153596602972414</v>
+      </c>
+      <c r="R26" s="225">
+        <f>Tabela2[[#This Row],[VWO_R]]*Tabela2[[#This Row],[VWD]]</f>
+        <v>1024.2120026574148</v>
+      </c>
+      <c r="S26" s="209">
+        <f>(Tabela2[[#This Row],[V_Def]]+Tabela2[[#This Row],[V_Off]])/2</f>
+        <v>551.68279963019359</v>
+      </c>
+      <c r="T26" s="209">
+        <f>472.09/Tabela2[[#This Row],[!ŚREDNIA]]</f>
+        <v>0.85572724093709895</v>
+      </c>
+      <c r="U26" s="209">
+        <f>Tabela2[[#This Row],[VWO]]+Tabela2[[#This Row],[VWD]]</f>
+        <v>39.284942791762013</v>
+      </c>
+      <c r="V26" s="209">
+        <f>Tabela2[[#This Row],[Suma VW]]*Tabela2[[#This Row],[Odchyłka]]</f>
+        <v>33.617195705566282</v>
+      </c>
+      <c r="W26" s="209">
+        <f>Tabela2[[#This Row],[Suma*Odchyłka]]/2*1.17</f>
+        <v>19.666059487756275</v>
+      </c>
+      <c r="X26" s="209">
+        <f>15000/Tabela2[[#This Row],[Kolumna2]]/27.17</f>
+        <v>28.072705657767123</v>
+      </c>
+      <c r="Y26" s="218">
+        <f>Tabela2[[#This Row],[!ŚREDNIA]]/MAX(Tabela2[!ŚREDNIA])</f>
+        <v>0.11693953197824576</v>
+      </c>
+      <c r="Z26" s="176">
+        <f>Tabela2[[#This Row],[VWO]]/Tabela2[[#This Row],[V_Off]]*1000</f>
+        <v>62.662976957053907</v>
+      </c>
+      <c r="AA26" s="176">
+        <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[V_Def]]*1000</f>
+        <v>33.513513513513516</v>
+      </c>
+      <c r="AB26" s="144">
+        <f>1/(AVERAGE((Tabela2[[#This Row],[Damage max]],Tabela2[[#This Row],[Damage min]]))*(1+(Tabela2[[#This Row],[Attack]]-$H$9)*IF(Tabela2[[#This Row],[Attack]]-$H$9 = 0, 1, IF(Tabela2[[#This Row],[Attack]]-$H$9 &gt; 0,$F$4,$I$4)))/$F$9)</f>
+        <v>108.04020100502511</v>
+      </c>
+      <c r="AC26" s="144">
+        <f>(AVERAGE($I$9,$J$9))*(1+(($G$9-Tabela2[[#This Row],[Defence]])*IF($G$9-Tabela2[[#This Row],[Defence]] = 0, 1, IF($G$9-Tabela2[[#This Row],[Defence]] &gt; 0, $F$4,$I$4))))/Tabela2[[#This Row],[Health]]</f>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="AD26" s="177">
+        <f>INT(SQRT(((Tabela2[[#This Row],[VWO]])*Tabela2[[#This Row],[VWD]])))</f>
+        <v>13</v>
+      </c>
+      <c r="AE26" s="176">
+        <f>Tabela2[[#This Row],[VWD]]/Tabela2[[#This Row],[VWO]]</f>
+        <v>6.9203513693068572</v>
+      </c>
+      <c r="AF26" s="218">
+        <f>Tabela2[[#This Row],[VOB]]/Tabela2[[#This Row],[VDB]]</f>
+        <v>24.932354078082721</v>
+      </c>
+      <c r="AG26" s="176">
+        <f>SUM(Tabela2[[#This Row],[Cena_Atak]:[Cena_Obrona]])</f>
+        <v>96.176490470567416</v>
+      </c>
+      <c r="AH26" s="176">
+        <f>300*Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]</f>
+        <v>870900</v>
+      </c>
+      <c r="AI26" s="248">
+        <v>2903</v>
+      </c>
+      <c r="AJ26" s="245">
+        <v>2522</v>
+      </c>
+      <c r="AK26" s="143">
+        <v>2900</v>
+      </c>
+      <c r="AL26" s="245">
+        <f>(Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching]]+Tabela2[[#This Row],[FixedAmountAfterSearchingFixedAmountAfterSearching2]]+Tabela2[[#This Row],[FixedAmountAfterSearching]])/3</f>
+        <v>2775</v>
+      </c>
+      <c r="AN26" s="141">
+        <f>Tabela2[[#This Row],[ŚREDNIA]]/136</f>
+        <v>20.404411764705884</v>
+      </c>
+      <c r="AO26" s="141">
+        <f t="shared" si="0"/>
+        <v>49.009009009009006</v>
+      </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="135"/>
       <c r="B27" s="135"/>
       <c r="C27" s="135"/>
@@ -6834,7 +7379,7 @@
       <c r="I27" s="135"/>
       <c r="J27" s="135"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="135"/>
       <c r="B28" s="135"/>
       <c r="C28" s="135"/>
@@ -6846,7 +7391,7 @@
       <c r="I28" s="135"/>
       <c r="J28" s="135"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="135"/>
       <c r="B29" s="135"/>
       <c r="C29" s="135"/>
@@ -6858,7 +7403,7 @@
       <c r="I29" s="135"/>
       <c r="J29" s="135"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="135"/>
       <c r="B30" s="135"/>
       <c r="C30" s="135"/>
@@ -6870,7 +7415,7 @@
       <c r="I30" s="135"/>
       <c r="J30" s="135"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="135"/>
       <c r="B31" s="135"/>
       <c r="C31" s="135"/>
@@ -6882,17 +7427,17 @@
       <c r="I31" s="135"/>
       <c r="J31" s="135"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="135"/>
       <c r="B32" s="135"/>
       <c r="C32" s="135"/>
       <c r="D32" s="135"/>
-      <c r="E32" s="138"/>
-      <c r="F32" s="138"/>
-      <c r="G32" s="138"/>
-      <c r="H32" s="138"/>
-      <c r="I32" s="138"/>
-      <c r="J32" s="138"/>
+      <c r="E32" s="135"/>
+      <c r="F32" s="135"/>
+      <c r="G32" s="135"/>
+      <c r="H32" s="135"/>
+      <c r="I32" s="135"/>
+      <c r="J32" s="135"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="135"/>
@@ -6911,7 +7456,7 @@
       <c r="B34" s="135"/>
       <c r="C34" s="135"/>
       <c r="D34" s="135"/>
-      <c r="E34" s="135"/>
+      <c r="E34" s="138"/>
       <c r="F34" s="138"/>
       <c r="G34" s="138"/>
       <c r="H34" s="138"/>
@@ -6978,29 +7523,41 @@
       <c r="I39" s="138"/>
       <c r="J39" s="138"/>
     </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="135"/>
+      <c r="B40" s="135"/>
+      <c r="C40" s="135"/>
+      <c r="D40" s="135"/>
+      <c r="E40" s="135"/>
+      <c r="F40" s="138"/>
+      <c r="G40" s="138"/>
+      <c r="H40" s="138"/>
+      <c r="I40" s="138"/>
+      <c r="J40" s="138"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="17" priority="6">
-      <formula>"Toster"</formula>
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Lizardman">
+      <formula>NOT(ISERROR(SEARCH("Lizardman",D1)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Barbarians">
+      <formula>NOT(ISERROR(SEARCH("Barbarians",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Toster">
+      <formula>NOT(ISERROR(SEARCH("Toster",D1)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>Toster</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$D$9</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4">
-      <formula>Toster</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Toster">
-      <formula>NOT(ISERROR(SEARCH("Toster",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="Barbarians">
-      <formula>NOT(ISERROR(SEARCH("Barbarians",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="Lizardman">
-      <formula>NOT(ISERROR(SEARCH("Lizardman",D1)))</formula>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>"Toster"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7013,13 +7570,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC138"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="T127" sqref="T127"/>
+      <selection pane="bottomLeft" activeCell="B118" sqref="A118:XFD118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18902,7 +19459,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B1:AD137">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:AD137">
     <sortCondition ref="AB1:AB137"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18910,7 +19467,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19231,7 +19788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>